<commit_message>
fix redundant empty lines
</commit_message>
<xml_diff>
--- a/25/Before_Soc_EEH2.xlsx
+++ b/25/Before_Soc_EEH2.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:AQ11"/>
+  <dimension ref="B1:AP11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:42">
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
@@ -582,7 +582,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:42">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -704,13 +704,10 @@
         <v>2.209176956159429</v>
       </c>
       <c r="AP2" t="n">
-        <v>28.22560354059191</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>4.650577989592598</v>
+        <v>1.480808714107192</v>
       </c>
     </row>
-    <row r="3" spans="1:43">
+    <row r="3" spans="1:42">
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
@@ -832,13 +829,10 @@
         <v>1.787431766817031</v>
       </c>
       <c r="AP3" t="n">
-        <v>10.57979310933031</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>5.587101763527078</v>
+        <v>0.8075663965570536</v>
       </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:42">
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
@@ -960,13 +954,10 @@
         <v>0.3279490906067143</v>
       </c>
       <c r="AP4" t="n">
-        <v>7.128908380986231</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>3.87693097095664</v>
+        <v>0.4025583646820428</v>
       </c>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:42">
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1088,13 +1079,10 @@
         <v>0.9085756914540868</v>
       </c>
       <c r="AP5" t="n">
-        <v>5.385218696082716</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>2.964421167601975</v>
+        <v>0.6899572908529897</v>
       </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:42">
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1216,13 +1204,10 @@
         <v>1.065821715104587</v>
       </c>
       <c r="AP6" t="n">
-        <v>7.114809759803852</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>2.499652195879408</v>
+        <v>0.5377756708469189</v>
       </c>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:42">
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1344,13 +1329,10 @@
         <v>5.950348025609667</v>
       </c>
       <c r="AP7" t="n">
-        <v>9.869715748413872</v>
-      </c>
-      <c r="AQ7" t="n">
-        <v>4.579847663476225</v>
+        <v>4.16202276582262</v>
       </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:42">
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1472,13 +1454,10 @@
         <v>0.4479854582717208</v>
       </c>
       <c r="AP8" t="n">
-        <v>15.38775535155383</v>
-      </c>
-      <c r="AQ8" t="n">
-        <v>8.668264346186257</v>
+        <v>0.4448370713058029</v>
       </c>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:42">
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1600,13 +1579,10 @@
         <v>3.635882482259043</v>
       </c>
       <c r="AP9" t="n">
-        <v>9.344731485578649</v>
-      </c>
-      <c r="AQ9" t="n">
-        <v>5.220975290224175</v>
+        <v>0.6166176369715476</v>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:42">
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1728,13 +1704,10 @@
         <v>0.3494206609082391</v>
       </c>
       <c r="AP10" t="n">
-        <v>5.533635385322023</v>
-      </c>
-      <c r="AQ10" t="n">
-        <v>2.155126514087637</v>
+        <v>0.1467987596757228</v>
       </c>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:42">
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1856,10 +1829,7 @@
         <v>0.2811929051568232</v>
       </c>
       <c r="AP11" t="n">
-        <v>14.59529836010645</v>
-      </c>
-      <c r="AQ11" t="n">
-        <v>4.482484280676183</v>
+        <v>0.2284570196298694</v>
       </c>
     </row>
   </sheetData>
@@ -1873,7 +1843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:AQ11"/>
+  <dimension ref="B1:AP11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1881,7 +1851,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:42">
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
@@ -2006,7 +1976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:42">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -2128,13 +2098,10 @@
         <v>5.988812833498085</v>
       </c>
       <c r="AP2" t="n">
-        <v>2.454809403065446</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.005768116218618937</v>
+        <v>5.81862352789444</v>
       </c>
     </row>
-    <row r="3" spans="1:43">
+    <row r="3" spans="1:42">
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
@@ -2256,13 +2223,10 @@
         <v>6.365917144071394</v>
       </c>
       <c r="AP3" t="n">
-        <v>3.364865597157544</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>0.01577634279244654</v>
+        <v>8.874440198440888</v>
       </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:42">
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
@@ -2384,13 +2348,10 @@
         <v>8.09068813395108</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.38763394499427</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>0.002537519485470378</v>
+        <v>8.39327524993538</v>
       </c>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:42">
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
@@ -2512,13 +2473,10 @@
         <v>7.667869411798966</v>
       </c>
       <c r="AP5" t="n">
-        <v>3.375625774954312</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>0.002536936577967821</v>
+        <v>8.219518966396434</v>
       </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:42">
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -2640,13 +2598,10 @@
         <v>5.049743314226872</v>
       </c>
       <c r="AP6" t="n">
-        <v>4.2997621174037</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>0.002536742337808863</v>
+        <v>6.815171239192523</v>
       </c>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:42">
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -2768,13 +2723,10 @@
         <v>8.970305823444425</v>
       </c>
       <c r="AP7" t="n">
-        <v>6.486799826332395</v>
-      </c>
-      <c r="AQ7" t="n">
-        <v>0.00253829713215286</v>
+        <v>8.578694557752547</v>
       </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:42">
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
@@ -2896,13 +2848,10 @@
         <v>7.019091496675265</v>
       </c>
       <c r="AP8" t="n">
-        <v>0.03652050872662742</v>
-      </c>
-      <c r="AQ8" t="n">
-        <v>0.00236943999420598</v>
+        <v>8.234669674043829</v>
       </c>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:42">
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
@@ -3024,13 +2973,10 @@
         <v>5.090426638823443</v>
       </c>
       <c r="AP9" t="n">
-        <v>1.720768838607268</v>
-      </c>
-      <c r="AQ9" t="n">
-        <v>0.002538686142779712</v>
+        <v>6.811470816989324</v>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:42">
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
@@ -3152,13 +3098,10 @@
         <v>9.344811526250112</v>
       </c>
       <c r="AP10" t="n">
-        <v>4.505844946148144</v>
-      </c>
-      <c r="AQ10" t="n">
-        <v>0.002369259797646739</v>
+        <v>7.450296224191622</v>
       </c>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:42">
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
@@ -3280,10 +3223,7 @@
         <v>7.851361519975502</v>
       </c>
       <c r="AP11" t="n">
-        <v>2.117278916872646</v>
-      </c>
-      <c r="AQ11" t="n">
-        <v>0.002539075278345081</v>
+        <v>7.330916878114602</v>
       </c>
     </row>
   </sheetData>
@@ -3297,7 +3237,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:AQ11"/>
+  <dimension ref="B1:AP11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3305,7 +3245,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:42">
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
@@ -3430,7 +3370,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:42">
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
@@ -3552,13 +3492,10 @@
         <v>0.576187949416508</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.6774444098422603</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.5407391309134406</v>
+        <v>0.6835320619646125</v>
       </c>
     </row>
-    <row r="3" spans="1:43">
+    <row r="3" spans="1:42">
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
@@ -3680,13 +3617,10 @@
         <v>0.6994738582643596</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.6313856725225175</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>0.5407420236292402</v>
+        <v>0.6316767355853479</v>
       </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:42">
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
@@ -3808,13 +3742,10 @@
         <v>0.7169929994007973</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.5611847908596858</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>0.5407436272197856</v>
+        <v>0.5613107430178561</v>
       </c>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:42">
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
@@ -3936,13 +3867,10 @@
         <v>0.7352683619771924</v>
       </c>
       <c r="AP5" t="n">
-        <v>0.6276859599497224</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>0.5407422570306015</v>
+        <v>0.6279557123376847</v>
       </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:42">
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
@@ -4064,13 +3992,10 @@
         <v>0.6729105214726948</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.5796263216674892</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>0.5407373304700513</v>
+        <v>0.5810877097758038</v>
       </c>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:42">
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -4192,13 +4117,10 @@
         <v>0.5823234225708563</v>
       </c>
       <c r="AP7" t="n">
-        <v>0.7290011872539199</v>
-      </c>
-      <c r="AQ7" t="n">
-        <v>0.5407444268834601</v>
+        <v>0.7294717938370332</v>
       </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:42">
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
@@ -4320,13 +4242,10 @@
         <v>0.6008631474547682</v>
       </c>
       <c r="AP8" t="n">
-        <v>0.5574907371022527</v>
-      </c>
-      <c r="AQ8" t="n">
-        <v>0.5407467849870082</v>
+        <v>0.5575697229131329</v>
       </c>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:42">
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
@@ -4448,13 +4367,10 @@
         <v>0.5563341359273007</v>
       </c>
       <c r="AP9" t="n">
-        <v>0.6307005410656747</v>
-      </c>
-      <c r="AQ9" t="n">
-        <v>0.5407458911428115</v>
+        <v>0.6311833169644426</v>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:42">
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
@@ -4576,13 +4492,10 @@
         <v>0.5797913098457796</v>
       </c>
       <c r="AP10" t="n">
-        <v>0.6464241020523772</v>
-      </c>
-      <c r="AQ10" t="n">
-        <v>0.5407464017613662</v>
+        <v>0.648578548383285</v>
       </c>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:42">
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
@@ -4704,10 +4617,7 @@
         <v>0.7512741906428894</v>
       </c>
       <c r="AP11" t="n">
-        <v>0.6391712158944118</v>
-      </c>
-      <c r="AQ11" t="n">
-        <v>0.540746771488003</v>
+        <v>0.6408262317860869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>